<commit_message>
Impor data, fixing user, fixing access
</commit_message>
<xml_diff>
--- a/tes_impor_data_pasien.xlsx
+++ b/tes_impor_data_pasien.xlsx
@@ -20,7 +20,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">Nomor RM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nama KK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tgl Lahir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No HP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jenis Kelamin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alamat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pendidikan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pekerjaan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sudah Menikah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alergi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kategori</t>
+  </si>
   <si>
     <t xml:space="preserve">A0001</t>
   </si>
@@ -29,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">Rozikin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-01-23</t>
   </si>
   <si>
     <t xml:space="preserve">-</t>
@@ -53,11 +95,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0"/>
-    <numFmt numFmtId="166" formatCode="0"/>
+    <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
     <numFmt numFmtId="167" formatCode="dd\ mmmm\ yyyy"/>
+    <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -132,25 +175,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -158,6 +197,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -178,74 +225,113 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="7.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="2.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="9.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="23.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="6.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="5.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="8.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="5.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="2.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="2.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="9.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="5.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="2.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="n">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="6" t="n">
-        <v>36914.2916666667</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>8</v>
+      <c r="M2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>